<commit_message>
Cập nhật đề 13
</commit_message>
<xml_diff>
--- a/Exports/Bài trắc nghiệm TACN_Split-100_4.xlsx
+++ b/Exports/Bài trắc nghiệm TACN_Split-100_4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="436">
   <si>
     <t>Câu hỏi</t>
   </si>
@@ -887,6 +887,441 @@
   </si>
   <si>
     <t>groups of people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A set of methods can be grouped together, ______ shared  variables, into a class.  </t>
+  </si>
+  <si>
+    <t>along within some</t>
+  </si>
+  <si>
+    <t>along some</t>
+  </si>
+  <si>
+    <t>along within</t>
+  </si>
+  <si>
+    <t>along with some</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In designing a user interface it is as well to realize  that there are several potentially different viewpoints. The perspectives  include </t>
+  </si>
+  <si>
+    <t>the end-user who will eventually get to use the software</t>
+  </si>
+  <si>
+    <t>the novice or occasional user</t>
+  </si>
+  <si>
+    <t>different end-users with different personalities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In various programming languages, a component is ______ </t>
+  </si>
+  <si>
+    <t>a method</t>
+  </si>
+  <si>
+    <t>a class</t>
+  </si>
+  <si>
+    <t>a package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A novice user or an occasional user______ remember much  about how to use the system.  </t>
+  </si>
+  <si>
+    <t>is not</t>
+  </si>
+  <si>
+    <t>is not likely to</t>
+  </si>
+  <si>
+    <t>are not likely to</t>
+  </si>
+  <si>
+    <t>is likely to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The skill level of the end user has a  significant impact on the ability to  </t>
+  </si>
+  <si>
+    <t>effectively apply heuristics that create a rhythm of interaction</t>
+  </si>
+  <si>
+    <t>respond efficiently to tasks that are demanded by the interaction</t>
+  </si>
+  <si>
+    <t>extract meaningful information from the user interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thus a direct manipulation interface______ suitable  approach.  </t>
+  </si>
+  <si>
+    <t>be the most</t>
+  </si>
+  <si>
+    <t>may be the most</t>
+  </si>
+  <si>
+    <t>may be most</t>
+  </si>
+  <si>
+    <t>may the most</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The scenario is  software ______ thousands or even hundreds of thousands of lines of code </t>
+  </si>
+  <si>
+    <t>that consists off</t>
+  </si>
+  <si>
+    <t>that consist of</t>
+  </si>
+  <si>
+    <t>that consists of</t>
+  </si>
+  <si>
+    <t>that consists in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems that context- or domain-specific knowledge  ______ overall education or intelligence. </t>
+  </si>
+  <si>
+    <t>is important than</t>
+  </si>
+  <si>
+    <t>is more important then</t>
+  </si>
+  <si>
+    <t>are more important than</t>
+  </si>
+  <si>
+    <t>is more important than</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a variety of mechanisms for splitting software  into independent components, or, expressed another way, grouping together items  ______ mutual affinity.  </t>
+  </si>
+  <si>
+    <t>that having some</t>
+  </si>
+  <si>
+    <t>that has sometimes</t>
+  </si>
+  <si>
+    <t>that has some</t>
+  </si>
+  <si>
+    <t>that have some</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This aim has consequences _____ stages of software  development, as follows.  </t>
+  </si>
+  <si>
+    <t>for nearly that all</t>
+  </si>
+  <si>
+    <t>for nearly all</t>
+  </si>
+  <si>
+    <t>for all that</t>
+  </si>
+  <si>
+    <t>for shall all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An interface used by two individuals with the  same education and background but entirely different personalities ______ and  unfriendly to the other.  </t>
+  </si>
+  <si>
+    <t>may seem friendly to one</t>
+  </si>
+  <si>
+    <t>may seem one</t>
+  </si>
+  <si>
+    <t>may saw to one</t>
+  </si>
+  <si>
+    <t>may see friendly for one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therefore, the ideal user interface would be designed to  accommodate differences in personality, or, alternatively, would be designed to  accommodate a typical personality ______.  </t>
+  </si>
+  <si>
+    <t>among a class of end users</t>
+  </si>
+  <si>
+    <t>a class of end users</t>
+  </si>
+  <si>
+    <t>among a class end users</t>
+  </si>
+  <si>
+    <t>classes of end users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the finest level of granularity, ______  statements and variable declarations can be placed in a method.  </t>
+  </si>
+  <si>
+    <t>a numbers of</t>
+  </si>
+  <si>
+    <t>a number of</t>
+  </si>
+  <si>
+    <t>number of</t>
+  </si>
+  <si>
+    <t>a number off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In designing a user interface it ______ realize that  there are several potentially different viewpoints. </t>
+  </si>
+  <si>
+    <t>is as good to</t>
+  </si>
+  <si>
+    <t>are good</t>
+  </si>
+  <si>
+    <t>is as well for</t>
+  </si>
+  <si>
+    <t>is as well to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The problem is that different people often have  different perspectives of the user interface; they also have different ______.  </t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>personalities</t>
+  </si>
+  <si>
+    <t>culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In essence, the desire for modularity ______  construct software from pieces that are as independent of each other as  possible.  </t>
+  </si>
+  <si>
+    <t>is trying to be</t>
+  </si>
+  <si>
+    <t>is about</t>
+  </si>
+  <si>
+    <t>is about trying to</t>
+  </si>
+  <si>
+    <t>is to trying to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For example, a number of applications provide a  macro facility, ______ commands can be grouped together, parameterized and  invoked as a single command </t>
+  </si>
+  <si>
+    <t>in which of</t>
+  </si>
+  <si>
+    <t>in which a series of</t>
+  </si>
+  <si>
+    <t>in series of</t>
+  </si>
+  <si>
+    <t>which a series of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most people do not apply any formal reasoning ______ a  problem, such as understanding what a computer is displaying.  </t>
+  </si>
+  <si>
+    <t>when matched with</t>
+  </si>
+  <si>
+    <t>confronting with</t>
+  </si>
+  <si>
+    <t>when confronted with</t>
+  </si>
+  <si>
+    <t>matching with</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ______ the desktop metaphor, familiar to users of  Microsoft and Apple Macintosh operating systems.  </t>
+  </si>
+  <si>
+    <t>best hidden of those are</t>
+  </si>
+  <si>
+    <t>not known of these is</t>
+  </si>
+  <si>
+    <t>best known of these is</t>
+  </si>
+  <si>
+    <t>best known of these are</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each person has some model ______ system works  and what it does. </t>
+  </si>
+  <si>
+    <t>of whereas the</t>
+  </si>
+  <si>
+    <t>of how the</t>
+  </si>
+  <si>
+    <t>of who the</t>
+  </si>
+  <si>
+    <t>of whom the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thus a component is a fairly independent piece of program  ______, some instructions and some data of its own. </t>
+  </si>
+  <si>
+    <t>that don’t has a name</t>
+  </si>
+  <si>
+    <t>that has a name</t>
+  </si>
+  <si>
+    <t>that has name</t>
+  </si>
+  <si>
+    <t>that have a name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These heuristics tend to be domain specific – an  identical problem, encountered in entirely different contexts, ______ applying  different heuristics </t>
+  </si>
+  <si>
+    <t>might be solved by</t>
+  </si>
+  <si>
+    <t>might be</t>
+  </si>
+  <si>
+    <t>might be solving by</t>
+  </si>
+  <si>
+    <t>might solve by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A third possibility ______ interface that is flexible and  can be used in different ways according to personality differences.  </t>
+  </si>
+  <si>
+    <t>are to create an</t>
+  </si>
+  <si>
+    <t>is create an</t>
+  </si>
+  <si>
+    <t>is to create a</t>
+  </si>
+  <si>
+    <t>is to create an</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These different perspectives ______ mental models </t>
+  </si>
+  <si>
+    <t>is called</t>
+  </si>
+  <si>
+    <t>is sometimes called</t>
+  </si>
+  <si>
+    <t>are sometimes called</t>
+  </si>
+  <si>
+    <t>are sometimes call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">But an experienced and frequent user may be  frustrated by an interface ______ novices and may prefer shortcut commands  and/or a command line interface </t>
+  </si>
+  <si>
+    <t>designed for</t>
+  </si>
+  <si>
+    <t>designing for</t>
+  </si>
+  <si>
+    <t>designed to</t>
+  </si>
+  <si>
+    <t>design for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While there is a massive trend towards multitasking,  window-oriented, point and pick interfaces which can make HCI easier, this  ______ careful design of the interface is conducted. </t>
+  </si>
+  <si>
+    <t>only detect</t>
+  </si>
+  <si>
+    <t>only happens</t>
+  </si>
+  <si>
+    <t>only happen if</t>
+  </si>
+  <si>
+    <t>only happens if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideally, each component should be self-contained and  ______ references as possible to other components.  </t>
+  </si>
+  <si>
+    <t>has as few</t>
+  </si>
+  <si>
+    <t>have few</t>
+  </si>
+  <si>
+    <t>has a few</t>
+  </si>
+  <si>
+    <t>have as few</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rather, they apply  a set of ______ based on their understanding of similar problems.  </t>
+  </si>
+  <si>
+    <t>strategies</t>
+  </si>
+  <si>
+    <t>rules</t>
+  </si>
+  <si>
+    <t>guidelines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For example, an engineer who uses a computer-based  diagnostic system ______ automobiles understands the problem domain and can  interact effectively through an interface specifically designed to accommodate  users with an engineer’s background. </t>
+  </si>
+  <si>
+    <t>to find a fault in</t>
+  </si>
+  <si>
+    <t>to finding faults in</t>
+  </si>
+  <si>
+    <t>to find faults in</t>
+  </si>
+  <si>
+    <t>to find faults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This same interface might confuse a physician, ______  physician has considerable experience of using a computer for diagnosing  illnesses in patients </t>
+  </si>
+  <si>
+    <t>even though the</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>even</t>
+  </si>
+  <si>
+    <t>though</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1669,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr/>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -2460,6 +2895,606 @@
         <v>290</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>291</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>292</v>
+      </c>
+      <c r="D62" t="s">
+        <v>293</v>
+      </c>
+      <c r="E62" t="s">
+        <v>294</v>
+      </c>
+      <c r="F62" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>297</v>
+      </c>
+      <c r="D63" t="s">
+        <v>298</v>
+      </c>
+      <c r="E63" t="s">
+        <v>299</v>
+      </c>
+      <c r="F63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>300</v>
+      </c>
+      <c r="B64" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" t="s">
+        <v>45</v>
+      </c>
+      <c r="D64" t="s">
+        <v>301</v>
+      </c>
+      <c r="E64" t="s">
+        <v>302</v>
+      </c>
+      <c r="F64" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>304</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" t="s">
+        <v>305</v>
+      </c>
+      <c r="D65" t="s">
+        <v>306</v>
+      </c>
+      <c r="E65" t="s">
+        <v>307</v>
+      </c>
+      <c r="F65" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>309</v>
+      </c>
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" t="s">
+        <v>45</v>
+      </c>
+      <c r="D66" t="s">
+        <v>310</v>
+      </c>
+      <c r="E66" t="s">
+        <v>311</v>
+      </c>
+      <c r="F66" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>313</v>
+      </c>
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" t="s">
+        <v>314</v>
+      </c>
+      <c r="D67" t="s">
+        <v>315</v>
+      </c>
+      <c r="E67" t="s">
+        <v>316</v>
+      </c>
+      <c r="F67" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>318</v>
+      </c>
+      <c r="B68" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" t="s">
+        <v>319</v>
+      </c>
+      <c r="D68" t="s">
+        <v>320</v>
+      </c>
+      <c r="E68" t="s">
+        <v>321</v>
+      </c>
+      <c r="F68" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>323</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
+        <v>324</v>
+      </c>
+      <c r="D69" t="s">
+        <v>325</v>
+      </c>
+      <c r="E69" t="s">
+        <v>326</v>
+      </c>
+      <c r="F69" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>328</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>329</v>
+      </c>
+      <c r="D70" t="s">
+        <v>330</v>
+      </c>
+      <c r="E70" t="s">
+        <v>331</v>
+      </c>
+      <c r="F70" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>333</v>
+      </c>
+      <c r="B71" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" t="s">
+        <v>334</v>
+      </c>
+      <c r="D71" t="s">
+        <v>335</v>
+      </c>
+      <c r="E71" t="s">
+        <v>336</v>
+      </c>
+      <c r="F71" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>338</v>
+      </c>
+      <c r="B72" t="s">
+        <v>93</v>
+      </c>
+      <c r="C72" t="s">
+        <v>339</v>
+      </c>
+      <c r="D72" t="s">
+        <v>340</v>
+      </c>
+      <c r="E72" t="s">
+        <v>341</v>
+      </c>
+      <c r="F72" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>343</v>
+      </c>
+      <c r="B73" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73" t="s">
+        <v>344</v>
+      </c>
+      <c r="D73" t="s">
+        <v>345</v>
+      </c>
+      <c r="E73" t="s">
+        <v>346</v>
+      </c>
+      <c r="F73" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>348</v>
+      </c>
+      <c r="B74" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" t="s">
+        <v>349</v>
+      </c>
+      <c r="D74" t="s">
+        <v>350</v>
+      </c>
+      <c r="E74" t="s">
+        <v>351</v>
+      </c>
+      <c r="F74" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>353</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>354</v>
+      </c>
+      <c r="D75" t="s">
+        <v>355</v>
+      </c>
+      <c r="E75" t="s">
+        <v>356</v>
+      </c>
+      <c r="F75" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>358</v>
+      </c>
+      <c r="B76" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" t="s">
+        <v>45</v>
+      </c>
+      <c r="D76" t="s">
+        <v>359</v>
+      </c>
+      <c r="E76" t="s">
+        <v>360</v>
+      </c>
+      <c r="F76" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>362</v>
+      </c>
+      <c r="B77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" t="s">
+        <v>363</v>
+      </c>
+      <c r="D77" t="s">
+        <v>364</v>
+      </c>
+      <c r="E77" t="s">
+        <v>365</v>
+      </c>
+      <c r="F77" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>367</v>
+      </c>
+      <c r="B78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" t="s">
+        <v>368</v>
+      </c>
+      <c r="D78" t="s">
+        <v>369</v>
+      </c>
+      <c r="E78" t="s">
+        <v>370</v>
+      </c>
+      <c r="F78" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>372</v>
+      </c>
+      <c r="B79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
+        <v>373</v>
+      </c>
+      <c r="D79" t="s">
+        <v>374</v>
+      </c>
+      <c r="E79" t="s">
+        <v>375</v>
+      </c>
+      <c r="F79" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>377</v>
+      </c>
+      <c r="B80" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" t="s">
+        <v>378</v>
+      </c>
+      <c r="D80" t="s">
+        <v>379</v>
+      </c>
+      <c r="E80" t="s">
+        <v>380</v>
+      </c>
+      <c r="F80" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>382</v>
+      </c>
+      <c r="B81" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" t="s">
+        <v>383</v>
+      </c>
+      <c r="D81" t="s">
+        <v>384</v>
+      </c>
+      <c r="E81" t="s">
+        <v>385</v>
+      </c>
+      <c r="F81" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>387</v>
+      </c>
+      <c r="B82" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" t="s">
+        <v>388</v>
+      </c>
+      <c r="D82" t="s">
+        <v>389</v>
+      </c>
+      <c r="E82" t="s">
+        <v>390</v>
+      </c>
+      <c r="F82" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>392</v>
+      </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83" t="s">
+        <v>393</v>
+      </c>
+      <c r="D83" t="s">
+        <v>394</v>
+      </c>
+      <c r="E83" t="s">
+        <v>395</v>
+      </c>
+      <c r="F83" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>397</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>398</v>
+      </c>
+      <c r="D84" t="s">
+        <v>399</v>
+      </c>
+      <c r="E84" t="s">
+        <v>400</v>
+      </c>
+      <c r="F84" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>402</v>
+      </c>
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>403</v>
+      </c>
+      <c r="D85" t="s">
+        <v>404</v>
+      </c>
+      <c r="E85" t="s">
+        <v>405</v>
+      </c>
+      <c r="F85" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>407</v>
+      </c>
+      <c r="B86" t="s">
+        <v>93</v>
+      </c>
+      <c r="C86" t="s">
+        <v>408</v>
+      </c>
+      <c r="D86" t="s">
+        <v>409</v>
+      </c>
+      <c r="E86" t="s">
+        <v>410</v>
+      </c>
+      <c r="F86" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>412</v>
+      </c>
+      <c r="B87" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s">
+        <v>413</v>
+      </c>
+      <c r="D87" t="s">
+        <v>414</v>
+      </c>
+      <c r="E87" t="s">
+        <v>415</v>
+      </c>
+      <c r="F87" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>417</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>418</v>
+      </c>
+      <c r="D88" t="s">
+        <v>419</v>
+      </c>
+      <c r="E88" t="s">
+        <v>420</v>
+      </c>
+      <c r="F88" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>422</v>
+      </c>
+      <c r="B89" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" t="s">
+        <v>423</v>
+      </c>
+      <c r="D89" t="s">
+        <v>424</v>
+      </c>
+      <c r="E89" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>426</v>
+      </c>
+      <c r="B90" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90" t="s">
+        <v>427</v>
+      </c>
+      <c r="D90" t="s">
+        <v>428</v>
+      </c>
+      <c r="E90" t="s">
+        <v>429</v>
+      </c>
+      <c r="F90" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>431</v>
+      </c>
+      <c r="B91" t="s">
+        <v>93</v>
+      </c>
+      <c r="C91" t="s">
+        <v>432</v>
+      </c>
+      <c r="D91" t="s">
+        <v>433</v>
+      </c>
+      <c r="E91" t="s">
+        <v>434</v>
+      </c>
+      <c r="F91" t="s">
+        <v>435</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup orientation="portrait" scale="100" paperSize="9" fitToWidth="0" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>

</xml_diff>